<commit_message>
update careerbuilder.py and result
</commit_message>
<xml_diff>
--- a/Result/jobstreet.xlsx
+++ b/Result/jobstreet.xlsx
@@ -1,15 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tranc\OneDrive\Documents\GitHub\PythonScrapJob\Result\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="1230" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$G$476</definedName>
+  </definedNames>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -21547,8 +21555,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -21611,6 +21619,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -21657,7 +21673,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -21689,9 +21705,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -21723,6 +21740,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -21898,14 +21916,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G476"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:G478"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A453" workbookViewId="0">
+      <selection activeCell="C479" sqref="C479"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="50.28515625" customWidth="1"/>
+    <col min="4" max="4" width="24.7109375" customWidth="1"/>
+    <col min="5" max="5" width="82" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -21925,7 +21951,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -21945,7 +21971,7 @@
         <v>1214</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -21968,7 +21994,7 @@
         <v>1215</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -21991,7 +22017,7 @@
         <v>1216</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -22014,7 +22040,7 @@
         <v>1217</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -22037,7 +22063,7 @@
         <v>1218</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -22060,7 +22086,7 @@
         <v>1219</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -22083,7 +22109,7 @@
         <v>1220</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -22106,7 +22132,7 @@
         <v>1220</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -22126,7 +22152,7 @@
         <v>1207</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -22149,7 +22175,7 @@
         <v>1221</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -22172,7 +22198,7 @@
         <v>1215</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -22195,7 +22221,7 @@
         <v>1222</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -22218,7 +22244,7 @@
         <v>1223</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -22241,7 +22267,7 @@
         <v>1222</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -22264,7 +22290,7 @@
         <v>1224</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -22287,7 +22313,7 @@
         <v>1225</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -22310,7 +22336,7 @@
         <v>1223</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -22333,7 +22359,7 @@
         <v>1226</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -22356,7 +22382,7 @@
         <v>1227</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -22379,7 +22405,7 @@
         <v>1227</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -22402,7 +22428,7 @@
         <v>1228</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -22425,7 +22451,7 @@
         <v>1216</v>
       </c>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -22448,7 +22474,7 @@
         <v>1222</v>
       </c>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -22471,7 +22497,7 @@
         <v>1219</v>
       </c>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -22494,7 +22520,7 @@
         <v>1216</v>
       </c>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -22517,7 +22543,7 @@
         <v>1216</v>
       </c>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -22540,7 +22566,7 @@
         <v>1221</v>
       </c>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -22563,7 +22589,7 @@
         <v>1221</v>
       </c>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>28</v>
       </c>
@@ -22586,7 +22612,7 @@
         <v>1229</v>
       </c>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -22609,7 +22635,7 @@
         <v>1230</v>
       </c>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>30</v>
       </c>
@@ -22632,7 +22658,7 @@
         <v>1231</v>
       </c>
     </row>
-    <row r="33" spans="1:7">
+    <row r="33" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>31</v>
       </c>
@@ -22655,7 +22681,7 @@
         <v>1231</v>
       </c>
     </row>
-    <row r="34" spans="1:7">
+    <row r="34" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>32</v>
       </c>
@@ -22678,7 +22704,7 @@
         <v>1232</v>
       </c>
     </row>
-    <row r="35" spans="1:7">
+    <row r="35" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>33</v>
       </c>
@@ -22701,7 +22727,7 @@
         <v>1233</v>
       </c>
     </row>
-    <row r="36" spans="1:7">
+    <row r="36" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>34</v>
       </c>
@@ -22724,7 +22750,7 @@
         <v>1215</v>
       </c>
     </row>
-    <row r="37" spans="1:7">
+    <row r="37" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>35</v>
       </c>
@@ -22747,7 +22773,7 @@
         <v>1222</v>
       </c>
     </row>
-    <row r="38" spans="1:7">
+    <row r="38" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>36</v>
       </c>
@@ -22770,7 +22796,7 @@
         <v>1215</v>
       </c>
     </row>
-    <row r="39" spans="1:7">
+    <row r="39" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>37</v>
       </c>
@@ -22793,7 +22819,7 @@
         <v>1231</v>
       </c>
     </row>
-    <row r="40" spans="1:7">
+    <row r="40" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>38</v>
       </c>
@@ -22816,7 +22842,7 @@
         <v>1234</v>
       </c>
     </row>
-    <row r="41" spans="1:7">
+    <row r="41" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>39</v>
       </c>
@@ -22839,7 +22865,7 @@
         <v>1233</v>
       </c>
     </row>
-    <row r="42" spans="1:7">
+    <row r="42" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>40</v>
       </c>
@@ -22862,7 +22888,7 @@
         <v>1234</v>
       </c>
     </row>
-    <row r="43" spans="1:7">
+    <row r="43" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>41</v>
       </c>
@@ -22885,7 +22911,7 @@
         <v>1222</v>
       </c>
     </row>
-    <row r="44" spans="1:7">
+    <row r="44" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>42</v>
       </c>
@@ -22908,7 +22934,7 @@
         <v>1233</v>
       </c>
     </row>
-    <row r="45" spans="1:7">
+    <row r="45" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>43</v>
       </c>
@@ -22931,7 +22957,7 @@
         <v>1222</v>
       </c>
     </row>
-    <row r="46" spans="1:7">
+    <row r="46" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>44</v>
       </c>
@@ -22954,7 +22980,7 @@
         <v>1222</v>
       </c>
     </row>
-    <row r="47" spans="1:7">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>45</v>
       </c>
@@ -22977,7 +23003,7 @@
         <v>1235</v>
       </c>
     </row>
-    <row r="48" spans="1:7">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>46</v>
       </c>
@@ -23000,7 +23026,7 @@
         <v>1235</v>
       </c>
     </row>
-    <row r="49" spans="1:7">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>47</v>
       </c>
@@ -23023,7 +23049,7 @@
         <v>1220</v>
       </c>
     </row>
-    <row r="50" spans="1:7">
+    <row r="50" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>48</v>
       </c>
@@ -23046,7 +23072,7 @@
         <v>1214</v>
       </c>
     </row>
-    <row r="51" spans="1:7">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>49</v>
       </c>
@@ -23069,7 +23095,7 @@
         <v>1216</v>
       </c>
     </row>
-    <row r="52" spans="1:7">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>50</v>
       </c>
@@ -23092,7 +23118,7 @@
         <v>1223</v>
       </c>
     </row>
-    <row r="53" spans="1:7">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>51</v>
       </c>
@@ -23115,7 +23141,7 @@
         <v>1215</v>
       </c>
     </row>
-    <row r="54" spans="1:7">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>52</v>
       </c>
@@ -23138,7 +23164,7 @@
         <v>1233</v>
       </c>
     </row>
-    <row r="55" spans="1:7">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>53</v>
       </c>
@@ -23161,7 +23187,7 @@
         <v>1232</v>
       </c>
     </row>
-    <row r="56" spans="1:7">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>54</v>
       </c>
@@ -23184,7 +23210,7 @@
         <v>1236</v>
       </c>
     </row>
-    <row r="57" spans="1:7">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>55</v>
       </c>
@@ -23207,7 +23233,7 @@
         <v>1218</v>
       </c>
     </row>
-    <row r="58" spans="1:7">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>56</v>
       </c>
@@ -23230,7 +23256,7 @@
         <v>1218</v>
       </c>
     </row>
-    <row r="59" spans="1:7">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>57</v>
       </c>
@@ -23253,7 +23279,7 @@
         <v>1237</v>
       </c>
     </row>
-    <row r="60" spans="1:7">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>58</v>
       </c>
@@ -23276,7 +23302,7 @@
         <v>1238</v>
       </c>
     </row>
-    <row r="61" spans="1:7">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>59</v>
       </c>
@@ -23299,7 +23325,7 @@
         <v>1239</v>
       </c>
     </row>
-    <row r="62" spans="1:7">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>60</v>
       </c>
@@ -23322,7 +23348,7 @@
         <v>1220</v>
       </c>
     </row>
-    <row r="63" spans="1:7">
+    <row r="63" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>61</v>
       </c>
@@ -23345,7 +23371,7 @@
         <v>1240</v>
       </c>
     </row>
-    <row r="64" spans="1:7">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>62</v>
       </c>
@@ -23368,7 +23394,7 @@
         <v>1220</v>
       </c>
     </row>
-    <row r="65" spans="1:7">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>63</v>
       </c>
@@ -23391,7 +23417,7 @@
         <v>1220</v>
       </c>
     </row>
-    <row r="66" spans="1:7">
+    <row r="66" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>64</v>
       </c>
@@ -23414,7 +23440,7 @@
         <v>1222</v>
       </c>
     </row>
-    <row r="67" spans="1:7">
+    <row r="67" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>65</v>
       </c>
@@ -23437,7 +23463,7 @@
         <v>1241</v>
       </c>
     </row>
-    <row r="68" spans="1:7">
+    <row r="68" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>66</v>
       </c>
@@ -23460,7 +23486,7 @@
         <v>1241</v>
       </c>
     </row>
-    <row r="69" spans="1:7">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>67</v>
       </c>
@@ -23480,7 +23506,7 @@
         <v>1242</v>
       </c>
     </row>
-    <row r="70" spans="1:7">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>68</v>
       </c>
@@ -23500,7 +23526,7 @@
         <v>1243</v>
       </c>
     </row>
-    <row r="71" spans="1:7">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>69</v>
       </c>
@@ -23523,7 +23549,7 @@
         <v>1244</v>
       </c>
     </row>
-    <row r="72" spans="1:7">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>70</v>
       </c>
@@ -23543,7 +23569,7 @@
         <v>1240</v>
       </c>
     </row>
-    <row r="73" spans="1:7">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>71</v>
       </c>
@@ -23566,7 +23592,7 @@
         <v>1222</v>
       </c>
     </row>
-    <row r="74" spans="1:7">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>72</v>
       </c>
@@ -23589,7 +23615,7 @@
         <v>1240</v>
       </c>
     </row>
-    <row r="75" spans="1:7">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>73</v>
       </c>
@@ -23609,7 +23635,7 @@
         <v>1218</v>
       </c>
     </row>
-    <row r="76" spans="1:7">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>74</v>
       </c>
@@ -23632,7 +23658,7 @@
         <v>1240</v>
       </c>
     </row>
-    <row r="77" spans="1:7">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>75</v>
       </c>
@@ -23655,7 +23681,7 @@
         <v>1245</v>
       </c>
     </row>
-    <row r="78" spans="1:7">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>76</v>
       </c>
@@ -23678,7 +23704,7 @@
         <v>1245</v>
       </c>
     </row>
-    <row r="79" spans="1:7">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>77</v>
       </c>
@@ -23701,7 +23727,7 @@
         <v>1245</v>
       </c>
     </row>
-    <row r="80" spans="1:7">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>78</v>
       </c>
@@ -23721,7 +23747,7 @@
         <v>1225</v>
       </c>
     </row>
-    <row r="81" spans="1:7">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>79</v>
       </c>
@@ -23744,7 +23770,7 @@
         <v>1223</v>
       </c>
     </row>
-    <row r="82" spans="1:7">
+    <row r="82" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>80</v>
       </c>
@@ -23767,7 +23793,7 @@
         <v>1233</v>
       </c>
     </row>
-    <row r="83" spans="1:7">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>81</v>
       </c>
@@ -23787,7 +23813,7 @@
         <v>1208</v>
       </c>
     </row>
-    <row r="84" spans="1:7">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>82</v>
       </c>
@@ -23810,7 +23836,7 @@
         <v>1246</v>
       </c>
     </row>
-    <row r="85" spans="1:7">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>83</v>
       </c>
@@ -23833,7 +23859,7 @@
         <v>1233</v>
       </c>
     </row>
-    <row r="86" spans="1:7">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <v>84</v>
       </c>
@@ -23856,7 +23882,7 @@
         <v>1223</v>
       </c>
     </row>
-    <row r="87" spans="1:7">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <v>85</v>
       </c>
@@ -23879,7 +23905,7 @@
         <v>1216</v>
       </c>
     </row>
-    <row r="88" spans="1:7">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <v>86</v>
       </c>
@@ -23902,7 +23928,7 @@
         <v>1228</v>
       </c>
     </row>
-    <row r="89" spans="1:7">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
         <v>87</v>
       </c>
@@ -23925,7 +23951,7 @@
         <v>1216</v>
       </c>
     </row>
-    <row r="90" spans="1:7">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
         <v>88</v>
       </c>
@@ -23948,7 +23974,7 @@
         <v>1233</v>
       </c>
     </row>
-    <row r="91" spans="1:7">
+    <row r="91" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
         <v>89</v>
       </c>
@@ -23971,7 +23997,7 @@
         <v>1235</v>
       </c>
     </row>
-    <row r="92" spans="1:7">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
         <v>90</v>
       </c>
@@ -23991,7 +24017,7 @@
         <v>1209</v>
       </c>
     </row>
-    <row r="93" spans="1:7">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
         <v>91</v>
       </c>
@@ -24014,7 +24040,7 @@
         <v>1227</v>
       </c>
     </row>
-    <row r="94" spans="1:7">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
         <v>92</v>
       </c>
@@ -24034,7 +24060,7 @@
         <v>1210</v>
       </c>
     </row>
-    <row r="95" spans="1:7">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
         <v>93</v>
       </c>
@@ -24057,7 +24083,7 @@
         <v>1219</v>
       </c>
     </row>
-    <row r="96" spans="1:7">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
         <v>94</v>
       </c>
@@ -24080,7 +24106,7 @@
         <v>1247</v>
       </c>
     </row>
-    <row r="97" spans="1:7">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
         <v>95</v>
       </c>
@@ -24100,7 +24126,7 @@
         <v>1229</v>
       </c>
     </row>
-    <row r="98" spans="1:7">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
         <v>96</v>
       </c>
@@ -24123,7 +24149,7 @@
         <v>1216</v>
       </c>
     </row>
-    <row r="99" spans="1:7">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
         <v>97</v>
       </c>
@@ -24146,7 +24172,7 @@
         <v>1215</v>
       </c>
     </row>
-    <row r="100" spans="1:7">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
         <v>98</v>
       </c>
@@ -24169,7 +24195,7 @@
         <v>1215</v>
       </c>
     </row>
-    <row r="101" spans="1:7">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
         <v>99</v>
       </c>
@@ -24192,7 +24218,7 @@
         <v>1215</v>
       </c>
     </row>
-    <row r="102" spans="1:7">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
         <v>100</v>
       </c>
@@ -24215,7 +24241,7 @@
         <v>1232</v>
       </c>
     </row>
-    <row r="103" spans="1:7">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
         <v>101</v>
       </c>
@@ -24238,7 +24264,7 @@
         <v>1232</v>
       </c>
     </row>
-    <row r="104" spans="1:7">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
         <v>102</v>
       </c>
@@ -24261,7 +24287,7 @@
         <v>1232</v>
       </c>
     </row>
-    <row r="105" spans="1:7">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
         <v>103</v>
       </c>
@@ -24284,7 +24310,7 @@
         <v>1232</v>
       </c>
     </row>
-    <row r="106" spans="1:7">
+    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
         <v>104</v>
       </c>
@@ -24307,7 +24333,7 @@
         <v>1232</v>
       </c>
     </row>
-    <row r="107" spans="1:7">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" s="1">
         <v>105</v>
       </c>
@@ -24330,7 +24356,7 @@
         <v>1247</v>
       </c>
     </row>
-    <row r="108" spans="1:7">
+    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
         <v>106</v>
       </c>
@@ -24353,7 +24379,7 @@
         <v>1233</v>
       </c>
     </row>
-    <row r="109" spans="1:7">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109" s="1">
         <v>107</v>
       </c>
@@ -24376,7 +24402,7 @@
         <v>1222</v>
       </c>
     </row>
-    <row r="110" spans="1:7">
+    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110" s="1">
         <v>108</v>
       </c>
@@ -24399,7 +24425,7 @@
         <v>1233</v>
       </c>
     </row>
-    <row r="111" spans="1:7">
+    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A111" s="1">
         <v>109</v>
       </c>
@@ -24422,7 +24448,7 @@
         <v>1248</v>
       </c>
     </row>
-    <row r="112" spans="1:7">
+    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A112" s="1">
         <v>110</v>
       </c>
@@ -24445,7 +24471,7 @@
         <v>1233</v>
       </c>
     </row>
-    <row r="113" spans="1:7">
+    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A113" s="1">
         <v>111</v>
       </c>
@@ -24468,7 +24494,7 @@
         <v>1248</v>
       </c>
     </row>
-    <row r="114" spans="1:7">
+    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A114" s="1">
         <v>112</v>
       </c>
@@ -24491,7 +24517,7 @@
         <v>1230</v>
       </c>
     </row>
-    <row r="115" spans="1:7">
+    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A115" s="1">
         <v>113</v>
       </c>
@@ -24514,7 +24540,7 @@
         <v>1219</v>
       </c>
     </row>
-    <row r="116" spans="1:7">
+    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A116" s="1">
         <v>114</v>
       </c>
@@ -24537,7 +24563,7 @@
         <v>1222</v>
       </c>
     </row>
-    <row r="117" spans="1:7">
+    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A117" s="1">
         <v>115</v>
       </c>
@@ -24560,7 +24586,7 @@
         <v>1247</v>
       </c>
     </row>
-    <row r="118" spans="1:7">
+    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A118" s="1">
         <v>116</v>
       </c>
@@ -24583,7 +24609,7 @@
         <v>1232</v>
       </c>
     </row>
-    <row r="119" spans="1:7">
+    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A119" s="1">
         <v>117</v>
       </c>
@@ -24606,7 +24632,7 @@
         <v>1233</v>
       </c>
     </row>
-    <row r="120" spans="1:7">
+    <row r="120" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120" s="1">
         <v>118</v>
       </c>
@@ -24629,7 +24655,7 @@
         <v>1235</v>
       </c>
     </row>
-    <row r="121" spans="1:7">
+    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A121" s="1">
         <v>119</v>
       </c>
@@ -24652,7 +24678,7 @@
         <v>1233</v>
       </c>
     </row>
-    <row r="122" spans="1:7">
+    <row r="122" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A122" s="1">
         <v>120</v>
       </c>
@@ -24675,7 +24701,7 @@
         <v>1235</v>
       </c>
     </row>
-    <row r="123" spans="1:7">
+    <row r="123" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A123" s="1">
         <v>121</v>
       </c>
@@ -24698,7 +24724,7 @@
         <v>1237</v>
       </c>
     </row>
-    <row r="124" spans="1:7">
+    <row r="124" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A124" s="1">
         <v>122</v>
       </c>
@@ -24721,7 +24747,7 @@
         <v>1235</v>
       </c>
     </row>
-    <row r="125" spans="1:7">
+    <row r="125" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A125" s="1">
         <v>123</v>
       </c>
@@ -24744,7 +24770,7 @@
         <v>1235</v>
       </c>
     </row>
-    <row r="126" spans="1:7">
+    <row r="126" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A126" s="1">
         <v>124</v>
       </c>
@@ -24767,7 +24793,7 @@
         <v>1235</v>
       </c>
     </row>
-    <row r="127" spans="1:7">
+    <row r="127" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A127" s="1">
         <v>125</v>
       </c>
@@ -24790,7 +24816,7 @@
         <v>1235</v>
       </c>
     </row>
-    <row r="128" spans="1:7">
+    <row r="128" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A128" s="1">
         <v>126</v>
       </c>
@@ -24813,7 +24839,7 @@
         <v>1235</v>
       </c>
     </row>
-    <row r="129" spans="1:7">
+    <row r="129" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A129" s="1">
         <v>127</v>
       </c>
@@ -24836,7 +24862,7 @@
         <v>1235</v>
       </c>
     </row>
-    <row r="130" spans="1:7">
+    <row r="130" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A130" s="1">
         <v>128</v>
       </c>
@@ -24859,7 +24885,7 @@
         <v>1235</v>
       </c>
     </row>
-    <row r="131" spans="1:7">
+    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A131" s="1">
         <v>129</v>
       </c>
@@ -24882,7 +24908,7 @@
         <v>1235</v>
       </c>
     </row>
-    <row r="132" spans="1:7">
+    <row r="132" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A132" s="1">
         <v>130</v>
       </c>
@@ -24905,7 +24931,7 @@
         <v>1235</v>
       </c>
     </row>
-    <row r="133" spans="1:7">
+    <row r="133" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A133" s="1">
         <v>131</v>
       </c>
@@ -24928,7 +24954,7 @@
         <v>1235</v>
       </c>
     </row>
-    <row r="134" spans="1:7">
+    <row r="134" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A134" s="1">
         <v>132</v>
       </c>
@@ -24951,7 +24977,7 @@
         <v>1235</v>
       </c>
     </row>
-    <row r="135" spans="1:7">
+    <row r="135" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A135" s="1">
         <v>133</v>
       </c>
@@ -24974,7 +25000,7 @@
         <v>1235</v>
       </c>
     </row>
-    <row r="136" spans="1:7">
+    <row r="136" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A136" s="1">
         <v>134</v>
       </c>
@@ -24997,7 +25023,7 @@
         <v>1235</v>
       </c>
     </row>
-    <row r="137" spans="1:7">
+    <row r="137" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A137" s="1">
         <v>135</v>
       </c>
@@ -25020,7 +25046,7 @@
         <v>1235</v>
       </c>
     </row>
-    <row r="138" spans="1:7">
+    <row r="138" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A138" s="1">
         <v>136</v>
       </c>
@@ -25043,7 +25069,7 @@
         <v>1235</v>
       </c>
     </row>
-    <row r="139" spans="1:7">
+    <row r="139" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A139" s="1">
         <v>137</v>
       </c>
@@ -25066,7 +25092,7 @@
         <v>1235</v>
       </c>
     </row>
-    <row r="140" spans="1:7">
+    <row r="140" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A140" s="1">
         <v>138</v>
       </c>
@@ -25089,7 +25115,7 @@
         <v>1235</v>
       </c>
     </row>
-    <row r="141" spans="1:7">
+    <row r="141" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A141" s="1">
         <v>139</v>
       </c>
@@ -25112,7 +25138,7 @@
         <v>1235</v>
       </c>
     </row>
-    <row r="142" spans="1:7">
+    <row r="142" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A142" s="1">
         <v>140</v>
       </c>
@@ -25135,7 +25161,7 @@
         <v>1235</v>
       </c>
     </row>
-    <row r="143" spans="1:7">
+    <row r="143" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A143" s="1">
         <v>141</v>
       </c>
@@ -25158,7 +25184,7 @@
         <v>1235</v>
       </c>
     </row>
-    <row r="144" spans="1:7">
+    <row r="144" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A144" s="1">
         <v>142</v>
       </c>
@@ -25181,7 +25207,7 @@
         <v>1240</v>
       </c>
     </row>
-    <row r="145" spans="1:7">
+    <row r="145" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A145" s="1">
         <v>143</v>
       </c>
@@ -25204,7 +25230,7 @@
         <v>1224</v>
       </c>
     </row>
-    <row r="146" spans="1:7">
+    <row r="146" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A146" s="1">
         <v>144</v>
       </c>
@@ -25227,7 +25253,7 @@
         <v>1236</v>
       </c>
     </row>
-    <row r="147" spans="1:7">
+    <row r="147" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A147" s="1">
         <v>145</v>
       </c>
@@ -25250,7 +25276,7 @@
         <v>1220</v>
       </c>
     </row>
-    <row r="148" spans="1:7">
+    <row r="148" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A148" s="1">
         <v>146</v>
       </c>
@@ -25273,7 +25299,7 @@
         <v>1240</v>
       </c>
     </row>
-    <row r="149" spans="1:7">
+    <row r="149" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A149" s="1">
         <v>147</v>
       </c>
@@ -25296,7 +25322,7 @@
         <v>1227</v>
       </c>
     </row>
-    <row r="150" spans="1:7">
+    <row r="150" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A150" s="1">
         <v>148</v>
       </c>
@@ -25319,7 +25345,7 @@
         <v>1227</v>
       </c>
     </row>
-    <row r="151" spans="1:7">
+    <row r="151" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A151" s="1">
         <v>149</v>
       </c>
@@ -25342,7 +25368,7 @@
         <v>1216</v>
       </c>
     </row>
-    <row r="152" spans="1:7">
+    <row r="152" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A152" s="1">
         <v>150</v>
       </c>
@@ -25365,7 +25391,7 @@
         <v>1227</v>
       </c>
     </row>
-    <row r="153" spans="1:7">
+    <row r="153" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A153" s="1">
         <v>151</v>
       </c>
@@ -25388,7 +25414,7 @@
         <v>1222</v>
       </c>
     </row>
-    <row r="154" spans="1:7">
+    <row r="154" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A154" s="1">
         <v>152</v>
       </c>
@@ -25411,7 +25437,7 @@
         <v>1233</v>
       </c>
     </row>
-    <row r="155" spans="1:7">
+    <row r="155" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A155" s="1">
         <v>153</v>
       </c>
@@ -25434,7 +25460,7 @@
         <v>1229</v>
       </c>
     </row>
-    <row r="156" spans="1:7">
+    <row r="156" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A156" s="1">
         <v>154</v>
       </c>
@@ -25457,7 +25483,7 @@
         <v>1233</v>
       </c>
     </row>
-    <row r="157" spans="1:7">
+    <row r="157" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A157" s="1">
         <v>155</v>
       </c>
@@ -25480,7 +25506,7 @@
         <v>1229</v>
       </c>
     </row>
-    <row r="158" spans="1:7">
+    <row r="158" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A158" s="1">
         <v>156</v>
       </c>
@@ -25503,7 +25529,7 @@
         <v>1222</v>
       </c>
     </row>
-    <row r="159" spans="1:7">
+    <row r="159" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A159" s="1">
         <v>157</v>
       </c>
@@ -25526,7 +25552,7 @@
         <v>1234</v>
       </c>
     </row>
-    <row r="160" spans="1:7">
+    <row r="160" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A160" s="1">
         <v>158</v>
       </c>
@@ -25549,7 +25575,7 @@
         <v>1229</v>
       </c>
     </row>
-    <row r="161" spans="1:7">
+    <row r="161" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A161" s="1">
         <v>159</v>
       </c>
@@ -25572,7 +25598,7 @@
         <v>1220</v>
       </c>
     </row>
-    <row r="162" spans="1:7">
+    <row r="162" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A162" s="1">
         <v>160</v>
       </c>
@@ -25595,7 +25621,7 @@
         <v>1233</v>
       </c>
     </row>
-    <row r="163" spans="1:7">
+    <row r="163" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A163" s="1">
         <v>161</v>
       </c>
@@ -25618,7 +25644,7 @@
         <v>1249</v>
       </c>
     </row>
-    <row r="164" spans="1:7">
+    <row r="164" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A164" s="1">
         <v>162</v>
       </c>
@@ -25641,7 +25667,7 @@
         <v>1224</v>
       </c>
     </row>
-    <row r="165" spans="1:7">
+    <row r="165" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A165" s="1">
         <v>163</v>
       </c>
@@ -25664,7 +25690,7 @@
         <v>1233</v>
       </c>
     </row>
-    <row r="166" spans="1:7">
+    <row r="166" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A166" s="1">
         <v>164</v>
       </c>
@@ -25687,7 +25713,7 @@
         <v>1233</v>
       </c>
     </row>
-    <row r="167" spans="1:7">
+    <row r="167" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A167" s="1">
         <v>165</v>
       </c>
@@ -25710,7 +25736,7 @@
         <v>1227</v>
       </c>
     </row>
-    <row r="168" spans="1:7">
+    <row r="168" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A168" s="1">
         <v>166</v>
       </c>
@@ -25733,7 +25759,7 @@
         <v>1242</v>
       </c>
     </row>
-    <row r="169" spans="1:7">
+    <row r="169" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A169" s="1">
         <v>167</v>
       </c>
@@ -25756,7 +25782,7 @@
         <v>1233</v>
       </c>
     </row>
-    <row r="170" spans="1:7">
+    <row r="170" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A170" s="1">
         <v>168</v>
       </c>
@@ -25779,7 +25805,7 @@
         <v>1248</v>
       </c>
     </row>
-    <row r="171" spans="1:7">
+    <row r="171" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A171" s="1">
         <v>169</v>
       </c>
@@ -25802,7 +25828,7 @@
         <v>1216</v>
       </c>
     </row>
-    <row r="172" spans="1:7">
+    <row r="172" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A172" s="1">
         <v>170</v>
       </c>
@@ -25825,7 +25851,7 @@
         <v>1243</v>
       </c>
     </row>
-    <row r="173" spans="1:7">
+    <row r="173" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A173" s="1">
         <v>171</v>
       </c>
@@ -25848,7 +25874,7 @@
         <v>1228</v>
       </c>
     </row>
-    <row r="174" spans="1:7">
+    <row r="174" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A174" s="1">
         <v>172</v>
       </c>
@@ -25871,7 +25897,7 @@
         <v>1214</v>
       </c>
     </row>
-    <row r="175" spans="1:7">
+    <row r="175" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A175" s="1">
         <v>173</v>
       </c>
@@ -25894,7 +25920,7 @@
         <v>1233</v>
       </c>
     </row>
-    <row r="176" spans="1:7">
+    <row r="176" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A176" s="1">
         <v>174</v>
       </c>
@@ -25917,7 +25943,7 @@
         <v>1245</v>
       </c>
     </row>
-    <row r="177" spans="1:7">
+    <row r="177" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A177" s="1">
         <v>175</v>
       </c>
@@ -25940,7 +25966,7 @@
         <v>1233</v>
       </c>
     </row>
-    <row r="178" spans="1:7">
+    <row r="178" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A178" s="1">
         <v>176</v>
       </c>
@@ -25963,7 +25989,7 @@
         <v>1216</v>
       </c>
     </row>
-    <row r="179" spans="1:7">
+    <row r="179" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A179" s="1">
         <v>177</v>
       </c>
@@ -25986,7 +26012,7 @@
         <v>1224</v>
       </c>
     </row>
-    <row r="180" spans="1:7">
+    <row r="180" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A180" s="1">
         <v>178</v>
       </c>
@@ -26009,7 +26035,7 @@
         <v>1233</v>
       </c>
     </row>
-    <row r="181" spans="1:7">
+    <row r="181" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A181" s="1">
         <v>179</v>
       </c>
@@ -26032,7 +26058,7 @@
         <v>1224</v>
       </c>
     </row>
-    <row r="182" spans="1:7">
+    <row r="182" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A182" s="1">
         <v>180</v>
       </c>
@@ -26055,7 +26081,7 @@
         <v>1224</v>
       </c>
     </row>
-    <row r="183" spans="1:7">
+    <row r="183" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A183" s="1">
         <v>181</v>
       </c>
@@ -26078,7 +26104,7 @@
         <v>1224</v>
       </c>
     </row>
-    <row r="184" spans="1:7">
+    <row r="184" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A184" s="1">
         <v>182</v>
       </c>
@@ -26101,7 +26127,7 @@
         <v>1220</v>
       </c>
     </row>
-    <row r="185" spans="1:7">
+    <row r="185" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A185" s="1">
         <v>183</v>
       </c>
@@ -26124,7 +26150,7 @@
         <v>1240</v>
       </c>
     </row>
-    <row r="186" spans="1:7">
+    <row r="186" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A186" s="1">
         <v>184</v>
       </c>
@@ -26147,7 +26173,7 @@
         <v>1218</v>
       </c>
     </row>
-    <row r="187" spans="1:7">
+    <row r="187" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A187" s="1">
         <v>185</v>
       </c>
@@ -26170,7 +26196,7 @@
         <v>1226</v>
       </c>
     </row>
-    <row r="188" spans="1:7">
+    <row r="188" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A188" s="1">
         <v>186</v>
       </c>
@@ -26193,7 +26219,7 @@
         <v>1216</v>
       </c>
     </row>
-    <row r="189" spans="1:7">
+    <row r="189" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A189" s="1">
         <v>187</v>
       </c>
@@ -26216,7 +26242,7 @@
         <v>1221</v>
       </c>
     </row>
-    <row r="190" spans="1:7">
+    <row r="190" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A190" s="1">
         <v>188</v>
       </c>
@@ -26239,7 +26265,7 @@
         <v>1215</v>
       </c>
     </row>
-    <row r="191" spans="1:7">
+    <row r="191" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A191" s="1">
         <v>189</v>
       </c>
@@ -26262,7 +26288,7 @@
         <v>1216</v>
       </c>
     </row>
-    <row r="192" spans="1:7">
+    <row r="192" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A192" s="1">
         <v>190</v>
       </c>
@@ -26285,7 +26311,7 @@
         <v>1246</v>
       </c>
     </row>
-    <row r="193" spans="1:7">
+    <row r="193" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A193" s="1">
         <v>191</v>
       </c>
@@ -26308,7 +26334,7 @@
         <v>1248</v>
       </c>
     </row>
-    <row r="194" spans="1:7">
+    <row r="194" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A194" s="1">
         <v>192</v>
       </c>
@@ -26331,7 +26357,7 @@
         <v>1248</v>
       </c>
     </row>
-    <row r="195" spans="1:7">
+    <row r="195" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A195" s="1">
         <v>193</v>
       </c>
@@ -26354,7 +26380,7 @@
         <v>1246</v>
       </c>
     </row>
-    <row r="196" spans="1:7">
+    <row r="196" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A196" s="1">
         <v>194</v>
       </c>
@@ -26377,7 +26403,7 @@
         <v>1246</v>
       </c>
     </row>
-    <row r="197" spans="1:7">
+    <row r="197" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A197" s="1">
         <v>195</v>
       </c>
@@ -26400,7 +26426,7 @@
         <v>1248</v>
       </c>
     </row>
-    <row r="198" spans="1:7">
+    <row r="198" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A198" s="1">
         <v>196</v>
       </c>
@@ -26423,7 +26449,7 @@
         <v>1229</v>
       </c>
     </row>
-    <row r="199" spans="1:7">
+    <row r="199" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A199" s="1">
         <v>197</v>
       </c>
@@ -26446,7 +26472,7 @@
         <v>1233</v>
       </c>
     </row>
-    <row r="200" spans="1:7">
+    <row r="200" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A200" s="1">
         <v>198</v>
       </c>
@@ -26469,7 +26495,7 @@
         <v>1230</v>
       </c>
     </row>
-    <row r="201" spans="1:7">
+    <row r="201" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A201" s="1">
         <v>199</v>
       </c>
@@ -26492,7 +26518,7 @@
         <v>1215</v>
       </c>
     </row>
-    <row r="202" spans="1:7">
+    <row r="202" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A202" s="1">
         <v>200</v>
       </c>
@@ -26515,7 +26541,7 @@
         <v>1230</v>
       </c>
     </row>
-    <row r="203" spans="1:7">
+    <row r="203" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A203" s="1">
         <v>201</v>
       </c>
@@ -26538,7 +26564,7 @@
         <v>1234</v>
       </c>
     </row>
-    <row r="204" spans="1:7">
+    <row r="204" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A204" s="1">
         <v>202</v>
       </c>
@@ -26561,7 +26587,7 @@
         <v>1215</v>
       </c>
     </row>
-    <row r="205" spans="1:7">
+    <row r="205" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A205" s="1">
         <v>203</v>
       </c>
@@ -26584,7 +26610,7 @@
         <v>1233</v>
       </c>
     </row>
-    <row r="206" spans="1:7">
+    <row r="206" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A206" s="1">
         <v>204</v>
       </c>
@@ -26607,7 +26633,7 @@
         <v>1232</v>
       </c>
     </row>
-    <row r="207" spans="1:7">
+    <row r="207" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A207" s="1">
         <v>205</v>
       </c>
@@ -26630,7 +26656,7 @@
         <v>1218</v>
       </c>
     </row>
-    <row r="208" spans="1:7">
+    <row r="208" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A208" s="1">
         <v>206</v>
       </c>
@@ -26653,7 +26679,7 @@
         <v>1233</v>
       </c>
     </row>
-    <row r="209" spans="1:7">
+    <row r="209" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A209" s="1">
         <v>207</v>
       </c>
@@ -26676,7 +26702,7 @@
         <v>1250</v>
       </c>
     </row>
-    <row r="210" spans="1:7">
+    <row r="210" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A210" s="1">
         <v>208</v>
       </c>
@@ -26699,7 +26725,7 @@
         <v>1233</v>
       </c>
     </row>
-    <row r="211" spans="1:7">
+    <row r="211" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A211" s="1">
         <v>209</v>
       </c>
@@ -26722,7 +26748,7 @@
         <v>1233</v>
       </c>
     </row>
-    <row r="212" spans="1:7">
+    <row r="212" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A212" s="1">
         <v>210</v>
       </c>
@@ -26745,7 +26771,7 @@
         <v>1233</v>
       </c>
     </row>
-    <row r="213" spans="1:7">
+    <row r="213" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A213" s="1">
         <v>211</v>
       </c>
@@ -26768,7 +26794,7 @@
         <v>1246</v>
       </c>
     </row>
-    <row r="214" spans="1:7">
+    <row r="214" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A214" s="1">
         <v>212</v>
       </c>
@@ -26791,7 +26817,7 @@
         <v>1222</v>
       </c>
     </row>
-    <row r="215" spans="1:7">
+    <row r="215" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A215" s="1">
         <v>213</v>
       </c>
@@ -26814,7 +26840,7 @@
         <v>1222</v>
       </c>
     </row>
-    <row r="216" spans="1:7">
+    <row r="216" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A216" s="1">
         <v>214</v>
       </c>
@@ -26837,7 +26863,7 @@
         <v>1233</v>
       </c>
     </row>
-    <row r="217" spans="1:7">
+    <row r="217" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A217" s="1">
         <v>215</v>
       </c>
@@ -26860,7 +26886,7 @@
         <v>1233</v>
       </c>
     </row>
-    <row r="218" spans="1:7">
+    <row r="218" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A218" s="1">
         <v>216</v>
       </c>
@@ -26883,7 +26909,7 @@
         <v>1251</v>
       </c>
     </row>
-    <row r="219" spans="1:7">
+    <row r="219" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A219" s="1">
         <v>217</v>
       </c>
@@ -26906,7 +26932,7 @@
         <v>1252</v>
       </c>
     </row>
-    <row r="220" spans="1:7">
+    <row r="220" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A220" s="1">
         <v>218</v>
       </c>
@@ -26929,7 +26955,7 @@
         <v>1233</v>
       </c>
     </row>
-    <row r="221" spans="1:7">
+    <row r="221" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A221" s="1">
         <v>219</v>
       </c>
@@ -26952,7 +26978,7 @@
         <v>1232</v>
       </c>
     </row>
-    <row r="222" spans="1:7">
+    <row r="222" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A222" s="1">
         <v>220</v>
       </c>
@@ -26975,7 +27001,7 @@
         <v>1240</v>
       </c>
     </row>
-    <row r="223" spans="1:7">
+    <row r="223" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A223" s="1">
         <v>221</v>
       </c>
@@ -26998,7 +27024,7 @@
         <v>1219</v>
       </c>
     </row>
-    <row r="224" spans="1:7">
+    <row r="224" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A224" s="1">
         <v>222</v>
       </c>
@@ -27021,7 +27047,7 @@
         <v>1224</v>
       </c>
     </row>
-    <row r="225" spans="1:7">
+    <row r="225" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A225" s="1">
         <v>223</v>
       </c>
@@ -27044,7 +27070,7 @@
         <v>1236</v>
       </c>
     </row>
-    <row r="226" spans="1:7">
+    <row r="226" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A226" s="1">
         <v>224</v>
       </c>
@@ -27067,7 +27093,7 @@
         <v>1236</v>
       </c>
     </row>
-    <row r="227" spans="1:7">
+    <row r="227" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A227" s="1">
         <v>225</v>
       </c>
@@ -27090,7 +27116,7 @@
         <v>1223</v>
       </c>
     </row>
-    <row r="228" spans="1:7">
+    <row r="228" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A228" s="1">
         <v>226</v>
       </c>
@@ -27113,7 +27139,7 @@
         <v>1223</v>
       </c>
     </row>
-    <row r="229" spans="1:7">
+    <row r="229" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A229" s="1">
         <v>227</v>
       </c>
@@ -27136,7 +27162,7 @@
         <v>1218</v>
       </c>
     </row>
-    <row r="230" spans="1:7">
+    <row r="230" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A230" s="1">
         <v>228</v>
       </c>
@@ -27159,7 +27185,7 @@
         <v>1218</v>
       </c>
     </row>
-    <row r="231" spans="1:7">
+    <row r="231" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A231" s="1">
         <v>229</v>
       </c>
@@ -27182,7 +27208,7 @@
         <v>1223</v>
       </c>
     </row>
-    <row r="232" spans="1:7">
+    <row r="232" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A232" s="1">
         <v>230</v>
       </c>
@@ -27205,7 +27231,7 @@
         <v>1226</v>
       </c>
     </row>
-    <row r="233" spans="1:7">
+    <row r="233" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A233" s="1">
         <v>231</v>
       </c>
@@ -27228,7 +27254,7 @@
         <v>1223</v>
       </c>
     </row>
-    <row r="234" spans="1:7">
+    <row r="234" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A234" s="1">
         <v>232</v>
       </c>
@@ -27251,7 +27277,7 @@
         <v>1226</v>
       </c>
     </row>
-    <row r="235" spans="1:7">
+    <row r="235" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A235" s="1">
         <v>233</v>
       </c>
@@ -27274,7 +27300,7 @@
         <v>1218</v>
       </c>
     </row>
-    <row r="236" spans="1:7">
+    <row r="236" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A236" s="1">
         <v>234</v>
       </c>
@@ -27297,7 +27323,7 @@
         <v>1246</v>
       </c>
     </row>
-    <row r="237" spans="1:7">
+    <row r="237" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A237" s="1">
         <v>235</v>
       </c>
@@ -27320,7 +27346,7 @@
         <v>1226</v>
       </c>
     </row>
-    <row r="238" spans="1:7">
+    <row r="238" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A238" s="1">
         <v>236</v>
       </c>
@@ -27343,7 +27369,7 @@
         <v>1219</v>
       </c>
     </row>
-    <row r="239" spans="1:7">
+    <row r="239" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A239" s="1">
         <v>237</v>
       </c>
@@ -27366,7 +27392,7 @@
         <v>1233</v>
       </c>
     </row>
-    <row r="240" spans="1:7">
+    <row r="240" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A240" s="1">
         <v>238</v>
       </c>
@@ -27389,7 +27415,7 @@
         <v>1233</v>
       </c>
     </row>
-    <row r="241" spans="1:7">
+    <row r="241" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A241" s="1">
         <v>239</v>
       </c>
@@ -27412,7 +27438,7 @@
         <v>1247</v>
       </c>
     </row>
-    <row r="242" spans="1:7">
+    <row r="242" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A242" s="1">
         <v>240</v>
       </c>
@@ -27435,7 +27461,7 @@
         <v>1232</v>
       </c>
     </row>
-    <row r="243" spans="1:7">
+    <row r="243" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A243" s="1">
         <v>241</v>
       </c>
@@ -27458,7 +27484,7 @@
         <v>1246</v>
       </c>
     </row>
-    <row r="244" spans="1:7">
+    <row r="244" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A244" s="1">
         <v>242</v>
       </c>
@@ -27481,7 +27507,7 @@
         <v>1222</v>
       </c>
     </row>
-    <row r="245" spans="1:7">
+    <row r="245" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A245" s="1">
         <v>243</v>
       </c>
@@ -27504,7 +27530,7 @@
         <v>1249</v>
       </c>
     </row>
-    <row r="246" spans="1:7">
+    <row r="246" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A246" s="1">
         <v>244</v>
       </c>
@@ -27527,7 +27553,7 @@
         <v>1242</v>
       </c>
     </row>
-    <row r="247" spans="1:7">
+    <row r="247" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A247" s="1">
         <v>245</v>
       </c>
@@ -27547,7 +27573,7 @@
         <v>1208</v>
       </c>
     </row>
-    <row r="248" spans="1:7">
+    <row r="248" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A248" s="1">
         <v>246</v>
       </c>
@@ -27567,7 +27593,7 @@
         <v>1253</v>
       </c>
     </row>
-    <row r="249" spans="1:7">
+    <row r="249" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A249" s="1">
         <v>247</v>
       </c>
@@ -27587,7 +27613,7 @@
         <v>1208</v>
       </c>
     </row>
-    <row r="250" spans="1:7">
+    <row r="250" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A250" s="1">
         <v>248</v>
       </c>
@@ -27607,7 +27633,7 @@
         <v>1236</v>
       </c>
     </row>
-    <row r="251" spans="1:7">
+    <row r="251" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A251" s="1">
         <v>249</v>
       </c>
@@ -27630,7 +27656,7 @@
         <v>1236</v>
       </c>
     </row>
-    <row r="252" spans="1:7">
+    <row r="252" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A252" s="1">
         <v>250</v>
       </c>
@@ -27653,7 +27679,7 @@
         <v>1236</v>
       </c>
     </row>
-    <row r="253" spans="1:7">
+    <row r="253" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A253" s="1">
         <v>251</v>
       </c>
@@ -27676,7 +27702,7 @@
         <v>1254</v>
       </c>
     </row>
-    <row r="254" spans="1:7">
+    <row r="254" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A254" s="1">
         <v>252</v>
       </c>
@@ -27699,7 +27725,7 @@
         <v>1218</v>
       </c>
     </row>
-    <row r="255" spans="1:7">
+    <row r="255" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A255" s="1">
         <v>253</v>
       </c>
@@ -27722,7 +27748,7 @@
         <v>1255</v>
       </c>
     </row>
-    <row r="256" spans="1:7">
+    <row r="256" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A256" s="1">
         <v>254</v>
       </c>
@@ -27745,7 +27771,7 @@
         <v>1226</v>
       </c>
     </row>
-    <row r="257" spans="1:7">
+    <row r="257" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A257" s="1">
         <v>255</v>
       </c>
@@ -27768,7 +27794,7 @@
         <v>1255</v>
       </c>
     </row>
-    <row r="258" spans="1:7">
+    <row r="258" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A258" s="1">
         <v>256</v>
       </c>
@@ -27791,7 +27817,7 @@
         <v>1255</v>
       </c>
     </row>
-    <row r="259" spans="1:7">
+    <row r="259" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A259" s="1">
         <v>257</v>
       </c>
@@ -27814,7 +27840,7 @@
         <v>1255</v>
       </c>
     </row>
-    <row r="260" spans="1:7">
+    <row r="260" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A260" s="1">
         <v>258</v>
       </c>
@@ -27837,7 +27863,7 @@
         <v>1255</v>
       </c>
     </row>
-    <row r="261" spans="1:7">
+    <row r="261" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A261" s="1">
         <v>259</v>
       </c>
@@ -27860,7 +27886,7 @@
         <v>1255</v>
       </c>
     </row>
-    <row r="262" spans="1:7">
+    <row r="262" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A262" s="1">
         <v>260</v>
       </c>
@@ -27883,7 +27909,7 @@
         <v>1255</v>
       </c>
     </row>
-    <row r="263" spans="1:7">
+    <row r="263" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A263" s="1">
         <v>261</v>
       </c>
@@ -27906,7 +27932,7 @@
         <v>1255</v>
       </c>
     </row>
-    <row r="264" spans="1:7">
+    <row r="264" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A264" s="1">
         <v>262</v>
       </c>
@@ -27929,7 +27955,7 @@
         <v>1255</v>
       </c>
     </row>
-    <row r="265" spans="1:7">
+    <row r="265" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A265" s="1">
         <v>263</v>
       </c>
@@ -27952,7 +27978,7 @@
         <v>1236</v>
       </c>
     </row>
-    <row r="266" spans="1:7">
+    <row r="266" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A266" s="1">
         <v>264</v>
       </c>
@@ -27975,7 +28001,7 @@
         <v>1255</v>
       </c>
     </row>
-    <row r="267" spans="1:7">
+    <row r="267" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A267" s="1">
         <v>265</v>
       </c>
@@ -27998,7 +28024,7 @@
         <v>1255</v>
       </c>
     </row>
-    <row r="268" spans="1:7">
+    <row r="268" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A268" s="1">
         <v>266</v>
       </c>
@@ -28018,7 +28044,7 @@
         <v>1236</v>
       </c>
     </row>
-    <row r="269" spans="1:7">
+    <row r="269" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A269" s="1">
         <v>267</v>
       </c>
@@ -28038,7 +28064,7 @@
         <v>1209</v>
       </c>
     </row>
-    <row r="270" spans="1:7">
+    <row r="270" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A270" s="1">
         <v>268</v>
       </c>
@@ -28061,7 +28087,7 @@
         <v>1217</v>
       </c>
     </row>
-    <row r="271" spans="1:7">
+    <row r="271" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A271" s="1">
         <v>269</v>
       </c>
@@ -28084,7 +28110,7 @@
         <v>1217</v>
       </c>
     </row>
-    <row r="272" spans="1:7">
+    <row r="272" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A272" s="1">
         <v>270</v>
       </c>
@@ -28104,7 +28130,7 @@
         <v>1236</v>
       </c>
     </row>
-    <row r="273" spans="1:7">
+    <row r="273" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A273" s="1">
         <v>271</v>
       </c>
@@ -28127,7 +28153,7 @@
         <v>1236</v>
       </c>
     </row>
-    <row r="274" spans="1:7">
+    <row r="274" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A274" s="1">
         <v>272</v>
       </c>
@@ -28150,7 +28176,7 @@
         <v>1224</v>
       </c>
     </row>
-    <row r="275" spans="1:7">
+    <row r="275" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A275" s="1">
         <v>273</v>
       </c>
@@ -28173,7 +28199,7 @@
         <v>1247</v>
       </c>
     </row>
-    <row r="276" spans="1:7">
+    <row r="276" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A276" s="1">
         <v>274</v>
       </c>
@@ -28196,7 +28222,7 @@
         <v>1252</v>
       </c>
     </row>
-    <row r="277" spans="1:7">
+    <row r="277" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A277" s="1">
         <v>275</v>
       </c>
@@ -28219,7 +28245,7 @@
         <v>1216</v>
       </c>
     </row>
-    <row r="278" spans="1:7">
+    <row r="278" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A278" s="1">
         <v>276</v>
       </c>
@@ -28242,7 +28268,7 @@
         <v>1214</v>
       </c>
     </row>
-    <row r="279" spans="1:7">
+    <row r="279" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A279" s="1">
         <v>277</v>
       </c>
@@ -28265,7 +28291,7 @@
         <v>1223</v>
       </c>
     </row>
-    <row r="280" spans="1:7">
+    <row r="280" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A280" s="1">
         <v>278</v>
       </c>
@@ -28288,7 +28314,7 @@
         <v>1216</v>
       </c>
     </row>
-    <row r="281" spans="1:7">
+    <row r="281" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A281" s="1">
         <v>279</v>
       </c>
@@ -28311,7 +28337,7 @@
         <v>1214</v>
       </c>
     </row>
-    <row r="282" spans="1:7">
+    <row r="282" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A282" s="1">
         <v>280</v>
       </c>
@@ -28331,7 +28357,7 @@
         <v>1235</v>
       </c>
     </row>
-    <row r="283" spans="1:7">
+    <row r="283" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A283" s="1">
         <v>281</v>
       </c>
@@ -28354,7 +28380,7 @@
         <v>1227</v>
       </c>
     </row>
-    <row r="284" spans="1:7">
+    <row r="284" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A284" s="1">
         <v>282</v>
       </c>
@@ -28377,7 +28403,7 @@
         <v>1218</v>
       </c>
     </row>
-    <row r="285" spans="1:7">
+    <row r="285" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A285" s="1">
         <v>283</v>
       </c>
@@ -28397,7 +28423,7 @@
         <v>1235</v>
       </c>
     </row>
-    <row r="286" spans="1:7">
+    <row r="286" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A286" s="1">
         <v>284</v>
       </c>
@@ -28420,7 +28446,7 @@
         <v>1218</v>
       </c>
     </row>
-    <row r="287" spans="1:7">
+    <row r="287" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A287" s="1">
         <v>285</v>
       </c>
@@ -28443,7 +28469,7 @@
         <v>1223</v>
       </c>
     </row>
-    <row r="288" spans="1:7">
+    <row r="288" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A288" s="1">
         <v>286</v>
       </c>
@@ -28466,7 +28492,7 @@
         <v>1218</v>
       </c>
     </row>
-    <row r="289" spans="1:7">
+    <row r="289" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A289" s="1">
         <v>287</v>
       </c>
@@ -28489,7 +28515,7 @@
         <v>1218</v>
       </c>
     </row>
-    <row r="290" spans="1:7">
+    <row r="290" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A290" s="1">
         <v>288</v>
       </c>
@@ -28512,7 +28538,7 @@
         <v>1218</v>
       </c>
     </row>
-    <row r="291" spans="1:7">
+    <row r="291" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A291" s="1">
         <v>289</v>
       </c>
@@ -28535,7 +28561,7 @@
         <v>1218</v>
       </c>
     </row>
-    <row r="292" spans="1:7">
+    <row r="292" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A292" s="1">
         <v>290</v>
       </c>
@@ -28558,7 +28584,7 @@
         <v>1218</v>
       </c>
     </row>
-    <row r="293" spans="1:7">
+    <row r="293" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A293" s="1">
         <v>291</v>
       </c>
@@ -28581,7 +28607,7 @@
         <v>1256</v>
       </c>
     </row>
-    <row r="294" spans="1:7">
+    <row r="294" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A294" s="1">
         <v>292</v>
       </c>
@@ -28604,7 +28630,7 @@
         <v>1248</v>
       </c>
     </row>
-    <row r="295" spans="1:7">
+    <row r="295" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A295" s="1">
         <v>293</v>
       </c>
@@ -28627,7 +28653,7 @@
         <v>1218</v>
       </c>
     </row>
-    <row r="296" spans="1:7">
+    <row r="296" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A296" s="1">
         <v>294</v>
       </c>
@@ -28650,7 +28676,7 @@
         <v>1218</v>
       </c>
     </row>
-    <row r="297" spans="1:7">
+    <row r="297" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A297" s="1">
         <v>295</v>
       </c>
@@ -28673,7 +28699,7 @@
         <v>1218</v>
       </c>
     </row>
-    <row r="298" spans="1:7">
+    <row r="298" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A298" s="1">
         <v>296</v>
       </c>
@@ -28696,7 +28722,7 @@
         <v>1218</v>
       </c>
     </row>
-    <row r="299" spans="1:7">
+    <row r="299" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A299" s="1">
         <v>297</v>
       </c>
@@ -28719,7 +28745,7 @@
         <v>1223</v>
       </c>
     </row>
-    <row r="300" spans="1:7">
+    <row r="300" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A300" s="1">
         <v>298</v>
       </c>
@@ -28742,7 +28768,7 @@
         <v>1223</v>
       </c>
     </row>
-    <row r="301" spans="1:7">
+    <row r="301" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A301" s="1">
         <v>299</v>
       </c>
@@ -28765,7 +28791,7 @@
         <v>1223</v>
       </c>
     </row>
-    <row r="302" spans="1:7">
+    <row r="302" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A302" s="1">
         <v>300</v>
       </c>
@@ -28788,7 +28814,7 @@
         <v>1218</v>
       </c>
     </row>
-    <row r="303" spans="1:7">
+    <row r="303" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A303" s="1">
         <v>301</v>
       </c>
@@ -28811,7 +28837,7 @@
         <v>1218</v>
       </c>
     </row>
-    <row r="304" spans="1:7">
+    <row r="304" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A304" s="1">
         <v>302</v>
       </c>
@@ -28834,7 +28860,7 @@
         <v>1218</v>
       </c>
     </row>
-    <row r="305" spans="1:7">
+    <row r="305" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A305" s="1">
         <v>303</v>
       </c>
@@ -28857,7 +28883,7 @@
         <v>1233</v>
       </c>
     </row>
-    <row r="306" spans="1:7">
+    <row r="306" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A306" s="1">
         <v>304</v>
       </c>
@@ -28880,7 +28906,7 @@
         <v>1231</v>
       </c>
     </row>
-    <row r="307" spans="1:7">
+    <row r="307" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A307" s="1">
         <v>305</v>
       </c>
@@ -28903,7 +28929,7 @@
         <v>1226</v>
       </c>
     </row>
-    <row r="308" spans="1:7">
+    <row r="308" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A308" s="1">
         <v>306</v>
       </c>
@@ -28926,7 +28952,7 @@
         <v>1232</v>
       </c>
     </row>
-    <row r="309" spans="1:7">
+    <row r="309" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A309" s="1">
         <v>307</v>
       </c>
@@ -28949,7 +28975,7 @@
         <v>1215</v>
       </c>
     </row>
-    <row r="310" spans="1:7">
+    <row r="310" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A310" s="1">
         <v>308</v>
       </c>
@@ -28972,7 +28998,7 @@
         <v>1231</v>
       </c>
     </row>
-    <row r="311" spans="1:7">
+    <row r="311" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A311" s="1">
         <v>309</v>
       </c>
@@ -28995,7 +29021,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="312" spans="1:7">
+    <row r="312" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A312" s="1">
         <v>310</v>
       </c>
@@ -29018,7 +29044,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="313" spans="1:7">
+    <row r="313" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A313" s="1">
         <v>311</v>
       </c>
@@ -29041,7 +29067,7 @@
         <v>1222</v>
       </c>
     </row>
-    <row r="314" spans="1:7">
+    <row r="314" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A314" s="1">
         <v>312</v>
       </c>
@@ -29064,7 +29090,7 @@
         <v>1233</v>
       </c>
     </row>
-    <row r="315" spans="1:7">
+    <row r="315" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A315" s="1">
         <v>313</v>
       </c>
@@ -29087,7 +29113,7 @@
         <v>1222</v>
       </c>
     </row>
-    <row r="316" spans="1:7">
+    <row r="316" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A316" s="1">
         <v>314</v>
       </c>
@@ -29110,7 +29136,7 @@
         <v>1233</v>
       </c>
     </row>
-    <row r="317" spans="1:7">
+    <row r="317" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A317" s="1">
         <v>315</v>
       </c>
@@ -29133,7 +29159,7 @@
         <v>1216</v>
       </c>
     </row>
-    <row r="318" spans="1:7">
+    <row r="318" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A318" s="1">
         <v>316</v>
       </c>
@@ -29156,7 +29182,7 @@
         <v>1219</v>
       </c>
     </row>
-    <row r="319" spans="1:7">
+    <row r="319" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A319" s="1">
         <v>317</v>
       </c>
@@ -29179,7 +29205,7 @@
         <v>1233</v>
       </c>
     </row>
-    <row r="320" spans="1:7">
+    <row r="320" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A320" s="1">
         <v>318</v>
       </c>
@@ -29202,7 +29228,7 @@
         <v>1222</v>
       </c>
     </row>
-    <row r="321" spans="1:7">
+    <row r="321" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A321" s="1">
         <v>319</v>
       </c>
@@ -29225,7 +29251,7 @@
         <v>1246</v>
       </c>
     </row>
-    <row r="322" spans="1:7">
+    <row r="322" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A322" s="1">
         <v>320</v>
       </c>
@@ -29248,7 +29274,7 @@
         <v>1222</v>
       </c>
     </row>
-    <row r="323" spans="1:7">
+    <row r="323" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A323" s="1">
         <v>321</v>
       </c>
@@ -29271,7 +29297,7 @@
         <v>1248</v>
       </c>
     </row>
-    <row r="324" spans="1:7">
+    <row r="324" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A324" s="1">
         <v>322</v>
       </c>
@@ -29294,7 +29320,7 @@
         <v>1232</v>
       </c>
     </row>
-    <row r="325" spans="1:7">
+    <row r="325" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A325" s="1">
         <v>323</v>
       </c>
@@ -29317,7 +29343,7 @@
         <v>1231</v>
       </c>
     </row>
-    <row r="326" spans="1:7">
+    <row r="326" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A326" s="1">
         <v>324</v>
       </c>
@@ -29340,7 +29366,7 @@
         <v>1215</v>
       </c>
     </row>
-    <row r="327" spans="1:7">
+    <row r="327" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A327" s="1">
         <v>325</v>
       </c>
@@ -29363,7 +29389,7 @@
         <v>1214</v>
       </c>
     </row>
-    <row r="328" spans="1:7">
+    <row r="328" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A328" s="1">
         <v>326</v>
       </c>
@@ -29386,7 +29412,7 @@
         <v>1214</v>
       </c>
     </row>
-    <row r="329" spans="1:7">
+    <row r="329" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A329" s="1">
         <v>327</v>
       </c>
@@ -29406,7 +29432,7 @@
         <v>1235</v>
       </c>
     </row>
-    <row r="330" spans="1:7">
+    <row r="330" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A330" s="1">
         <v>328</v>
       </c>
@@ -29429,7 +29455,7 @@
         <v>1248</v>
       </c>
     </row>
-    <row r="331" spans="1:7">
+    <row r="331" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A331" s="1">
         <v>329</v>
       </c>
@@ -29452,7 +29478,7 @@
         <v>1246</v>
       </c>
     </row>
-    <row r="332" spans="1:7">
+    <row r="332" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A332" s="1">
         <v>330</v>
       </c>
@@ -29475,7 +29501,7 @@
         <v>1215</v>
       </c>
     </row>
-    <row r="333" spans="1:7">
+    <row r="333" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A333" s="1">
         <v>331</v>
       </c>
@@ -29498,7 +29524,7 @@
         <v>1214</v>
       </c>
     </row>
-    <row r="334" spans="1:7">
+    <row r="334" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A334" s="1">
         <v>332</v>
       </c>
@@ -29521,7 +29547,7 @@
         <v>1216</v>
       </c>
     </row>
-    <row r="335" spans="1:7">
+    <row r="335" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A335" s="1">
         <v>333</v>
       </c>
@@ -29544,7 +29570,7 @@
         <v>1214</v>
       </c>
     </row>
-    <row r="336" spans="1:7">
+    <row r="336" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A336" s="1">
         <v>334</v>
       </c>
@@ -29567,7 +29593,7 @@
         <v>1237</v>
       </c>
     </row>
-    <row r="337" spans="1:7">
+    <row r="337" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A337" s="1">
         <v>335</v>
       </c>
@@ -29590,7 +29616,7 @@
         <v>1256</v>
       </c>
     </row>
-    <row r="338" spans="1:7">
+    <row r="338" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A338" s="1">
         <v>336</v>
       </c>
@@ -29613,7 +29639,7 @@
         <v>1256</v>
       </c>
     </row>
-    <row r="339" spans="1:7">
+    <row r="339" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A339" s="1">
         <v>337</v>
       </c>
@@ -29636,7 +29662,7 @@
         <v>1256</v>
       </c>
     </row>
-    <row r="340" spans="1:7">
+    <row r="340" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A340" s="1">
         <v>338</v>
       </c>
@@ -29659,7 +29685,7 @@
         <v>1256</v>
       </c>
     </row>
-    <row r="341" spans="1:7">
+    <row r="341" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A341" s="1">
         <v>339</v>
       </c>
@@ -29682,7 +29708,7 @@
         <v>1229</v>
       </c>
     </row>
-    <row r="342" spans="1:7">
+    <row r="342" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A342" s="1">
         <v>340</v>
       </c>
@@ -29705,7 +29731,7 @@
         <v>1233</v>
       </c>
     </row>
-    <row r="343" spans="1:7">
+    <row r="343" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A343" s="1">
         <v>341</v>
       </c>
@@ -29728,7 +29754,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="344" spans="1:7">
+    <row r="344" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A344" s="1">
         <v>342</v>
       </c>
@@ -29751,7 +29777,7 @@
         <v>1259</v>
       </c>
     </row>
-    <row r="345" spans="1:7">
+    <row r="345" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A345" s="1">
         <v>343</v>
       </c>
@@ -29771,7 +29797,7 @@
         <v>1211</v>
       </c>
     </row>
-    <row r="346" spans="1:7">
+    <row r="346" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A346" s="1">
         <v>344</v>
       </c>
@@ -29794,7 +29820,7 @@
         <v>1222</v>
       </c>
     </row>
-    <row r="347" spans="1:7">
+    <row r="347" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A347" s="1">
         <v>345</v>
       </c>
@@ -29814,7 +29840,7 @@
         <v>1260</v>
       </c>
     </row>
-    <row r="348" spans="1:7">
+    <row r="348" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A348" s="1">
         <v>346</v>
       </c>
@@ -29834,7 +29860,7 @@
         <v>1260</v>
       </c>
     </row>
-    <row r="349" spans="1:7">
+    <row r="349" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A349" s="1">
         <v>347</v>
       </c>
@@ -29854,7 +29880,7 @@
         <v>1260</v>
       </c>
     </row>
-    <row r="350" spans="1:7">
+    <row r="350" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A350" s="1">
         <v>348</v>
       </c>
@@ -29877,7 +29903,7 @@
         <v>1259</v>
       </c>
     </row>
-    <row r="351" spans="1:7">
+    <row r="351" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A351" s="1">
         <v>349</v>
       </c>
@@ -29900,7 +29926,7 @@
         <v>1238</v>
       </c>
     </row>
-    <row r="352" spans="1:7">
+    <row r="352" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A352" s="1">
         <v>350</v>
       </c>
@@ -29923,7 +29949,7 @@
         <v>1240</v>
       </c>
     </row>
-    <row r="353" spans="1:7">
+    <row r="353" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A353" s="1">
         <v>351</v>
       </c>
@@ -29946,7 +29972,7 @@
         <v>1260</v>
       </c>
     </row>
-    <row r="354" spans="1:7">
+    <row r="354" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A354" s="1">
         <v>352</v>
       </c>
@@ -29966,7 +29992,7 @@
         <v>1235</v>
       </c>
     </row>
-    <row r="355" spans="1:7">
+    <row r="355" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A355" s="1">
         <v>353</v>
       </c>
@@ -29989,7 +30015,7 @@
         <v>1233</v>
       </c>
     </row>
-    <row r="356" spans="1:7">
+    <row r="356" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A356" s="1">
         <v>354</v>
       </c>
@@ -30012,7 +30038,7 @@
         <v>1233</v>
       </c>
     </row>
-    <row r="357" spans="1:7">
+    <row r="357" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A357" s="1">
         <v>355</v>
       </c>
@@ -30035,7 +30061,7 @@
         <v>1233</v>
       </c>
     </row>
-    <row r="358" spans="1:7">
+    <row r="358" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A358" s="1">
         <v>356</v>
       </c>
@@ -30058,7 +30084,7 @@
         <v>1233</v>
       </c>
     </row>
-    <row r="359" spans="1:7">
+    <row r="359" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A359" s="1">
         <v>357</v>
       </c>
@@ -30081,7 +30107,7 @@
         <v>1218</v>
       </c>
     </row>
-    <row r="360" spans="1:7">
+    <row r="360" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A360" s="1">
         <v>358</v>
       </c>
@@ -30104,7 +30130,7 @@
         <v>1233</v>
       </c>
     </row>
-    <row r="361" spans="1:7">
+    <row r="361" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A361" s="1">
         <v>359</v>
       </c>
@@ -30127,7 +30153,7 @@
         <v>1242</v>
       </c>
     </row>
-    <row r="362" spans="1:7">
+    <row r="362" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A362" s="1">
         <v>360</v>
       </c>
@@ -30150,7 +30176,7 @@
         <v>1233</v>
       </c>
     </row>
-    <row r="363" spans="1:7">
+    <row r="363" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A363" s="1">
         <v>361</v>
       </c>
@@ -30170,7 +30196,7 @@
         <v>1209</v>
       </c>
     </row>
-    <row r="364" spans="1:7">
+    <row r="364" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A364" s="1">
         <v>362</v>
       </c>
@@ -30193,7 +30219,7 @@
         <v>1246</v>
       </c>
     </row>
-    <row r="365" spans="1:7">
+    <row r="365" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A365" s="1">
         <v>363</v>
       </c>
@@ -30216,7 +30242,7 @@
         <v>1261</v>
       </c>
     </row>
-    <row r="366" spans="1:7">
+    <row r="366" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A366" s="1">
         <v>364</v>
       </c>
@@ -30239,7 +30265,7 @@
         <v>1243</v>
       </c>
     </row>
-    <row r="367" spans="1:7">
+    <row r="367" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A367" s="1">
         <v>365</v>
       </c>
@@ -30262,7 +30288,7 @@
         <v>1214</v>
       </c>
     </row>
-    <row r="368" spans="1:7">
+    <row r="368" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A368" s="1">
         <v>366</v>
       </c>
@@ -30285,7 +30311,7 @@
         <v>1226</v>
       </c>
     </row>
-    <row r="369" spans="1:7">
+    <row r="369" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A369" s="1">
         <v>367</v>
       </c>
@@ -30308,7 +30334,7 @@
         <v>1226</v>
       </c>
     </row>
-    <row r="370" spans="1:7">
+    <row r="370" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A370" s="1">
         <v>368</v>
       </c>
@@ -30331,7 +30357,7 @@
         <v>1219</v>
       </c>
     </row>
-    <row r="371" spans="1:7">
+    <row r="371" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A371" s="1">
         <v>369</v>
       </c>
@@ -30354,7 +30380,7 @@
         <v>1214</v>
       </c>
     </row>
-    <row r="372" spans="1:7">
+    <row r="372" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A372" s="1">
         <v>370</v>
       </c>
@@ -30377,7 +30403,7 @@
         <v>1262</v>
       </c>
     </row>
-    <row r="373" spans="1:7">
+    <row r="373" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A373" s="1">
         <v>371</v>
       </c>
@@ -30400,7 +30426,7 @@
         <v>1227</v>
       </c>
     </row>
-    <row r="374" spans="1:7">
+    <row r="374" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A374" s="1">
         <v>372</v>
       </c>
@@ -30423,7 +30449,7 @@
         <v>1227</v>
       </c>
     </row>
-    <row r="375" spans="1:7">
+    <row r="375" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A375" s="1">
         <v>373</v>
       </c>
@@ -30446,7 +30472,7 @@
         <v>1218</v>
       </c>
     </row>
-    <row r="376" spans="1:7">
+    <row r="376" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A376" s="1">
         <v>374</v>
       </c>
@@ -30469,7 +30495,7 @@
         <v>1233</v>
       </c>
     </row>
-    <row r="377" spans="1:7">
+    <row r="377" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A377" s="1">
         <v>375</v>
       </c>
@@ -30492,7 +30518,7 @@
         <v>1263</v>
       </c>
     </row>
-    <row r="378" spans="1:7">
+    <row r="378" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A378" s="1">
         <v>376</v>
       </c>
@@ -30515,7 +30541,7 @@
         <v>1219</v>
       </c>
     </row>
-    <row r="379" spans="1:7">
+    <row r="379" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A379" s="1">
         <v>377</v>
       </c>
@@ -30538,7 +30564,7 @@
         <v>1214</v>
       </c>
     </row>
-    <row r="380" spans="1:7">
+    <row r="380" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A380" s="1">
         <v>378</v>
       </c>
@@ -30561,7 +30587,7 @@
         <v>1233</v>
       </c>
     </row>
-    <row r="381" spans="1:7">
+    <row r="381" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A381" s="1">
         <v>379</v>
       </c>
@@ -30584,7 +30610,7 @@
         <v>1239</v>
       </c>
     </row>
-    <row r="382" spans="1:7">
+    <row r="382" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A382" s="1">
         <v>380</v>
       </c>
@@ -30607,7 +30633,7 @@
         <v>1251</v>
       </c>
     </row>
-    <row r="383" spans="1:7">
+    <row r="383" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A383" s="1">
         <v>381</v>
       </c>
@@ -30630,7 +30656,7 @@
         <v>1263</v>
       </c>
     </row>
-    <row r="384" spans="1:7">
+    <row r="384" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A384" s="1">
         <v>382</v>
       </c>
@@ -30650,7 +30676,7 @@
         <v>1210</v>
       </c>
     </row>
-    <row r="385" spans="1:7">
+    <row r="385" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A385" s="1">
         <v>383</v>
       </c>
@@ -30670,7 +30696,7 @@
         <v>1211</v>
       </c>
     </row>
-    <row r="386" spans="1:7">
+    <row r="386" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A386" s="1">
         <v>384</v>
       </c>
@@ -30690,7 +30716,7 @@
         <v>1224</v>
       </c>
     </row>
-    <row r="387" spans="1:7">
+    <row r="387" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A387" s="1">
         <v>385</v>
       </c>
@@ -30710,7 +30736,7 @@
         <v>1224</v>
       </c>
     </row>
-    <row r="388" spans="1:7">
+    <row r="388" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A388" s="1">
         <v>386</v>
       </c>
@@ -30733,7 +30759,7 @@
         <v>1224</v>
       </c>
     </row>
-    <row r="389" spans="1:7">
+    <row r="389" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A389" s="1">
         <v>387</v>
       </c>
@@ -30756,7 +30782,7 @@
         <v>1224</v>
       </c>
     </row>
-    <row r="390" spans="1:7">
+    <row r="390" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A390" s="1">
         <v>388</v>
       </c>
@@ -30776,7 +30802,7 @@
         <v>1209</v>
       </c>
     </row>
-    <row r="391" spans="1:7">
+    <row r="391" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A391" s="1">
         <v>389</v>
       </c>
@@ -30799,7 +30825,7 @@
         <v>1224</v>
       </c>
     </row>
-    <row r="392" spans="1:7">
+    <row r="392" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A392" s="1">
         <v>390</v>
       </c>
@@ -30822,7 +30848,7 @@
         <v>1224</v>
       </c>
     </row>
-    <row r="393" spans="1:7">
+    <row r="393" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A393" s="1">
         <v>391</v>
       </c>
@@ -30842,7 +30868,7 @@
         <v>1240</v>
       </c>
     </row>
-    <row r="394" spans="1:7">
+    <row r="394" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A394" s="1">
         <v>392</v>
       </c>
@@ -30865,7 +30891,7 @@
         <v>1224</v>
       </c>
     </row>
-    <row r="395" spans="1:7">
+    <row r="395" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A395" s="1">
         <v>393</v>
       </c>
@@ -30888,7 +30914,7 @@
         <v>1240</v>
       </c>
     </row>
-    <row r="396" spans="1:7">
+    <row r="396" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A396" s="1">
         <v>394</v>
       </c>
@@ -30911,7 +30937,7 @@
         <v>1224</v>
       </c>
     </row>
-    <row r="397" spans="1:7">
+    <row r="397" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A397" s="1">
         <v>395</v>
       </c>
@@ -30934,7 +30960,7 @@
         <v>1240</v>
       </c>
     </row>
-    <row r="398" spans="1:7">
+    <row r="398" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A398" s="1">
         <v>396</v>
       </c>
@@ -30957,7 +30983,7 @@
         <v>1263</v>
       </c>
     </row>
-    <row r="399" spans="1:7">
+    <row r="399" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A399" s="1">
         <v>397</v>
       </c>
@@ -30980,7 +31006,7 @@
         <v>1240</v>
       </c>
     </row>
-    <row r="400" spans="1:7">
+    <row r="400" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A400" s="1">
         <v>398</v>
       </c>
@@ -31003,7 +31029,7 @@
         <v>1240</v>
       </c>
     </row>
-    <row r="401" spans="1:7">
+    <row r="401" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A401" s="1">
         <v>399</v>
       </c>
@@ -31026,7 +31052,7 @@
         <v>1240</v>
       </c>
     </row>
-    <row r="402" spans="1:7">
+    <row r="402" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A402" s="1">
         <v>400</v>
       </c>
@@ -31049,7 +31075,7 @@
         <v>1224</v>
       </c>
     </row>
-    <row r="403" spans="1:7">
+    <row r="403" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A403" s="1">
         <v>401</v>
       </c>
@@ -31069,7 +31095,7 @@
         <v>1223</v>
       </c>
     </row>
-    <row r="404" spans="1:7">
+    <row r="404" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A404" s="1">
         <v>402</v>
       </c>
@@ -31092,7 +31118,7 @@
         <v>1224</v>
       </c>
     </row>
-    <row r="405" spans="1:7">
+    <row r="405" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A405" s="1">
         <v>403</v>
       </c>
@@ -31115,7 +31141,7 @@
         <v>1224</v>
       </c>
     </row>
-    <row r="406" spans="1:7">
+    <row r="406" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A406" s="1">
         <v>404</v>
       </c>
@@ -31138,7 +31164,7 @@
         <v>1240</v>
       </c>
     </row>
-    <row r="407" spans="1:7">
+    <row r="407" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A407" s="1">
         <v>405</v>
       </c>
@@ -31161,7 +31187,7 @@
         <v>1240</v>
       </c>
     </row>
-    <row r="408" spans="1:7">
+    <row r="408" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A408" s="1">
         <v>406</v>
       </c>
@@ -31181,7 +31207,7 @@
         <v>1207</v>
       </c>
     </row>
-    <row r="409" spans="1:7">
+    <row r="409" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A409" s="1">
         <v>407</v>
       </c>
@@ -31201,7 +31227,7 @@
         <v>1207</v>
       </c>
     </row>
-    <row r="410" spans="1:7">
+    <row r="410" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A410" s="1">
         <v>408</v>
       </c>
@@ -31221,7 +31247,7 @@
         <v>1223</v>
       </c>
     </row>
-    <row r="411" spans="1:7">
+    <row r="411" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A411" s="1">
         <v>409</v>
       </c>
@@ -31244,7 +31270,7 @@
         <v>1245</v>
       </c>
     </row>
-    <row r="412" spans="1:7">
+    <row r="412" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A412" s="1">
         <v>410</v>
       </c>
@@ -31264,7 +31290,7 @@
         <v>1208</v>
       </c>
     </row>
-    <row r="413" spans="1:7">
+    <row r="413" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A413" s="1">
         <v>411</v>
       </c>
@@ -31287,7 +31313,7 @@
         <v>1240</v>
       </c>
     </row>
-    <row r="414" spans="1:7">
+    <row r="414" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A414" s="1">
         <v>412</v>
       </c>
@@ -31310,7 +31336,7 @@
         <v>1240</v>
       </c>
     </row>
-    <row r="415" spans="1:7">
+    <row r="415" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A415" s="1">
         <v>413</v>
       </c>
@@ -31333,7 +31359,7 @@
         <v>1240</v>
       </c>
     </row>
-    <row r="416" spans="1:7">
+    <row r="416" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A416" s="1">
         <v>414</v>
       </c>
@@ -31356,7 +31382,7 @@
         <v>1240</v>
       </c>
     </row>
-    <row r="417" spans="1:7">
+    <row r="417" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A417" s="1">
         <v>415</v>
       </c>
@@ -31379,7 +31405,7 @@
         <v>1220</v>
       </c>
     </row>
-    <row r="418" spans="1:7">
+    <row r="418" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A418" s="1">
         <v>416</v>
       </c>
@@ -31402,7 +31428,7 @@
         <v>1223</v>
       </c>
     </row>
-    <row r="419" spans="1:7">
+    <row r="419" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A419" s="1">
         <v>417</v>
       </c>
@@ -31422,7 +31448,7 @@
         <v>1209</v>
       </c>
     </row>
-    <row r="420" spans="1:7">
+    <row r="420" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A420" s="1">
         <v>418</v>
       </c>
@@ -31445,7 +31471,7 @@
         <v>1245</v>
       </c>
     </row>
-    <row r="421" spans="1:7">
+    <row r="421" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A421" s="1">
         <v>419</v>
       </c>
@@ -31465,7 +31491,7 @@
         <v>1209</v>
       </c>
     </row>
-    <row r="422" spans="1:7">
+    <row r="422" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A422" s="1">
         <v>420</v>
       </c>
@@ -31485,7 +31511,7 @@
         <v>1226</v>
       </c>
     </row>
-    <row r="423" spans="1:7">
+    <row r="423" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A423" s="1">
         <v>421</v>
       </c>
@@ -31505,7 +31531,7 @@
         <v>1209</v>
       </c>
     </row>
-    <row r="424" spans="1:7">
+    <row r="424" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A424" s="1">
         <v>422</v>
       </c>
@@ -31528,7 +31554,7 @@
         <v>1240</v>
       </c>
     </row>
-    <row r="425" spans="1:7">
+    <row r="425" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A425" s="1">
         <v>423</v>
       </c>
@@ -31551,7 +31577,7 @@
         <v>1246</v>
       </c>
     </row>
-    <row r="426" spans="1:7">
+    <row r="426" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A426" s="1">
         <v>424</v>
       </c>
@@ -31574,7 +31600,7 @@
         <v>1255</v>
       </c>
     </row>
-    <row r="427" spans="1:7">
+    <row r="427" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A427" s="1">
         <v>425</v>
       </c>
@@ -31597,7 +31623,7 @@
         <v>1255</v>
       </c>
     </row>
-    <row r="428" spans="1:7">
+    <row r="428" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A428" s="1">
         <v>426</v>
       </c>
@@ -31617,7 +31643,7 @@
         <v>1212</v>
       </c>
     </row>
-    <row r="429" spans="1:7">
+    <row r="429" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A429" s="1">
         <v>427</v>
       </c>
@@ -31640,7 +31666,7 @@
         <v>1226</v>
       </c>
     </row>
-    <row r="430" spans="1:7">
+    <row r="430" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A430" s="1">
         <v>428</v>
       </c>
@@ -31660,7 +31686,7 @@
         <v>1213</v>
       </c>
     </row>
-    <row r="431" spans="1:7">
+    <row r="431" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A431" s="1">
         <v>429</v>
       </c>
@@ -31680,7 +31706,7 @@
         <v>1226</v>
       </c>
     </row>
-    <row r="432" spans="1:7">
+    <row r="432" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A432" s="1">
         <v>430</v>
       </c>
@@ -31703,7 +31729,7 @@
         <v>1220</v>
       </c>
     </row>
-    <row r="433" spans="1:7">
+    <row r="433" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A433" s="1">
         <v>431</v>
       </c>
@@ -31726,7 +31752,7 @@
         <v>1245</v>
       </c>
     </row>
-    <row r="434" spans="1:7">
+    <row r="434" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A434" s="1">
         <v>432</v>
       </c>
@@ -31746,7 +31772,7 @@
         <v>1216</v>
       </c>
     </row>
-    <row r="435" spans="1:7">
+    <row r="435" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A435" s="1">
         <v>433</v>
       </c>
@@ -31766,7 +31792,7 @@
         <v>1221</v>
       </c>
     </row>
-    <row r="436" spans="1:7">
+    <row r="436" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A436" s="1">
         <v>434</v>
       </c>
@@ -31786,7 +31812,7 @@
         <v>1216</v>
       </c>
     </row>
-    <row r="437" spans="1:7">
+    <row r="437" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A437" s="1">
         <v>435</v>
       </c>
@@ -31809,7 +31835,7 @@
         <v>1246</v>
       </c>
     </row>
-    <row r="438" spans="1:7">
+    <row r="438" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A438" s="1">
         <v>436</v>
       </c>
@@ -31832,7 +31858,7 @@
         <v>1227</v>
       </c>
     </row>
-    <row r="439" spans="1:7">
+    <row r="439" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A439" s="1">
         <v>437</v>
       </c>
@@ -31855,7 +31881,7 @@
         <v>1220</v>
       </c>
     </row>
-    <row r="440" spans="1:7">
+    <row r="440" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A440" s="1">
         <v>438</v>
       </c>
@@ -31878,7 +31904,7 @@
         <v>1227</v>
       </c>
     </row>
-    <row r="441" spans="1:7">
+    <row r="441" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A441" s="1">
         <v>439</v>
       </c>
@@ -31901,7 +31927,7 @@
         <v>1246</v>
       </c>
     </row>
-    <row r="442" spans="1:7">
+    <row r="442" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A442" s="1">
         <v>440</v>
       </c>
@@ -31921,7 +31947,7 @@
         <v>1210</v>
       </c>
     </row>
-    <row r="443" spans="1:7">
+    <row r="443" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A443" s="1">
         <v>441</v>
       </c>
@@ -31944,7 +31970,7 @@
         <v>1227</v>
       </c>
     </row>
-    <row r="444" spans="1:7">
+    <row r="444" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A444" s="1">
         <v>442</v>
       </c>
@@ -31967,7 +31993,7 @@
         <v>1216</v>
       </c>
     </row>
-    <row r="445" spans="1:7">
+    <row r="445" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A445" s="1">
         <v>443</v>
       </c>
@@ -31987,7 +32013,7 @@
         <v>1208</v>
       </c>
     </row>
-    <row r="446" spans="1:7">
+    <row r="446" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A446" s="1">
         <v>444</v>
       </c>
@@ -32010,7 +32036,7 @@
         <v>1227</v>
       </c>
     </row>
-    <row r="447" spans="1:7">
+    <row r="447" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A447" s="1">
         <v>445</v>
       </c>
@@ -32033,7 +32059,7 @@
         <v>1243</v>
       </c>
     </row>
-    <row r="448" spans="1:7">
+    <row r="448" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A448" s="1">
         <v>446</v>
       </c>
@@ -32056,7 +32082,7 @@
         <v>1227</v>
       </c>
     </row>
-    <row r="449" spans="1:7">
+    <row r="449" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A449" s="1">
         <v>447</v>
       </c>
@@ -32079,7 +32105,7 @@
         <v>1220</v>
       </c>
     </row>
-    <row r="450" spans="1:7">
+    <row r="450" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A450" s="1">
         <v>448</v>
       </c>
@@ -32102,7 +32128,7 @@
         <v>1246</v>
       </c>
     </row>
-    <row r="451" spans="1:7">
+    <row r="451" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A451" s="1">
         <v>449</v>
       </c>
@@ -32122,7 +32148,7 @@
         <v>1222</v>
       </c>
     </row>
-    <row r="452" spans="1:7">
+    <row r="452" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A452" s="1">
         <v>450</v>
       </c>
@@ -32145,7 +32171,7 @@
         <v>1219</v>
       </c>
     </row>
-    <row r="453" spans="1:7">
+    <row r="453" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A453" s="1">
         <v>451</v>
       </c>
@@ -32168,7 +32194,7 @@
         <v>1227</v>
       </c>
     </row>
-    <row r="454" spans="1:7">
+    <row r="454" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A454" s="1">
         <v>452</v>
       </c>
@@ -32191,7 +32217,7 @@
         <v>1220</v>
       </c>
     </row>
-    <row r="455" spans="1:7">
+    <row r="455" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A455" s="1">
         <v>453</v>
       </c>
@@ -32214,7 +32240,7 @@
         <v>1247</v>
       </c>
     </row>
-    <row r="456" spans="1:7">
+    <row r="456" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A456" s="1">
         <v>454</v>
       </c>
@@ -32237,7 +32263,7 @@
         <v>1214</v>
       </c>
     </row>
-    <row r="457" spans="1:7">
+    <row r="457" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A457" s="1">
         <v>455</v>
       </c>
@@ -32260,7 +32286,7 @@
         <v>1233</v>
       </c>
     </row>
-    <row r="458" spans="1:7">
+    <row r="458" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A458" s="1">
         <v>456</v>
       </c>
@@ -32283,7 +32309,7 @@
         <v>1227</v>
       </c>
     </row>
-    <row r="459" spans="1:7">
+    <row r="459" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A459" s="1">
         <v>457</v>
       </c>
@@ -32303,7 +32329,7 @@
         <v>1216</v>
       </c>
     </row>
-    <row r="460" spans="1:7">
+    <row r="460" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A460" s="1">
         <v>458</v>
       </c>
@@ -32326,7 +32352,7 @@
         <v>1228</v>
       </c>
     </row>
-    <row r="461" spans="1:7">
+    <row r="461" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A461" s="1">
         <v>459</v>
       </c>
@@ -32349,7 +32375,7 @@
         <v>1246</v>
       </c>
     </row>
-    <row r="462" spans="1:7">
+    <row r="462" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A462" s="1">
         <v>460</v>
       </c>
@@ -32369,7 +32395,7 @@
         <v>1233</v>
       </c>
     </row>
-    <row r="463" spans="1:7">
+    <row r="463" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A463" s="1">
         <v>461</v>
       </c>
@@ -32392,7 +32418,7 @@
         <v>1219</v>
       </c>
     </row>
-    <row r="464" spans="1:7">
+    <row r="464" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A464" s="1">
         <v>462</v>
       </c>
@@ -32415,7 +32441,7 @@
         <v>1233</v>
       </c>
     </row>
-    <row r="465" spans="1:7">
+    <row r="465" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A465" s="1">
         <v>463</v>
       </c>
@@ -32438,7 +32464,7 @@
         <v>1248</v>
       </c>
     </row>
-    <row r="466" spans="1:7">
+    <row r="466" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A466" s="1">
         <v>464</v>
       </c>
@@ -32461,7 +32487,7 @@
         <v>1233</v>
       </c>
     </row>
-    <row r="467" spans="1:7">
+    <row r="467" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A467" s="1">
         <v>465</v>
       </c>
@@ -32484,7 +32510,7 @@
         <v>1246</v>
       </c>
     </row>
-    <row r="468" spans="1:7">
+    <row r="468" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A468" s="1">
         <v>466</v>
       </c>
@@ -32507,7 +32533,7 @@
         <v>1229</v>
       </c>
     </row>
-    <row r="469" spans="1:7">
+    <row r="469" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A469" s="1">
         <v>467</v>
       </c>
@@ -32530,7 +32556,7 @@
         <v>1218</v>
       </c>
     </row>
-    <row r="470" spans="1:7">
+    <row r="470" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A470" s="1">
         <v>468</v>
       </c>
@@ -32553,7 +32579,7 @@
         <v>1214</v>
       </c>
     </row>
-    <row r="471" spans="1:7">
+    <row r="471" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A471" s="1">
         <v>469</v>
       </c>
@@ -32576,7 +32602,7 @@
         <v>1246</v>
       </c>
     </row>
-    <row r="472" spans="1:7">
+    <row r="472" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A472" s="1">
         <v>470</v>
       </c>
@@ -32599,7 +32625,7 @@
         <v>1214</v>
       </c>
     </row>
-    <row r="473" spans="1:7">
+    <row r="473" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A473" s="1">
         <v>471</v>
       </c>
@@ -32622,7 +32648,7 @@
         <v>1264</v>
       </c>
     </row>
-    <row r="474" spans="1:7">
+    <row r="474" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A474" s="1">
         <v>472</v>
       </c>
@@ -32645,7 +32671,7 @@
         <v>1246</v>
       </c>
     </row>
-    <row r="475" spans="1:7">
+    <row r="475" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A475" s="1">
         <v>473</v>
       </c>
@@ -32668,7 +32694,7 @@
         <v>1227</v>
       </c>
     </row>
-    <row r="476" spans="1:7">
+    <row r="476" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A476" s="1">
         <v>474</v>
       </c>
@@ -32691,7 +32717,21 @@
         <v>1214</v>
       </c>
     </row>
+    <row r="478" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C478">
+        <f>COUNTIF(C2:C476,"*data**anal*")</f>
+        <v>43</v>
+      </c>
+    </row>
   </sheetData>
+  <autoFilter ref="A1:G476">
+    <filterColumn colId="2">
+      <customFilters and="1">
+        <customFilter val="**data**"/>
+        <customFilter operator="notEqual" val="*database*"/>
+      </customFilters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>